<commit_message>
Added all testing doc files
</commit_message>
<xml_diff>
--- a/4.MONITORING AND CONTROLLING PHASE/Testing and Evaluating/Admin PHP/ADMIN PHP TESTING.xlsx
+++ b/4.MONITORING AND CONTROLLING PHASE/Testing and Evaluating/Admin PHP/ADMIN PHP TESTING.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flex\Desktop\Team-Portfolio\4.MONITORING AND CONTROLLING PHASE\Testing and Evaluating\Admin PHP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\Portfolio Team Project\Team-Portfolio\4.MONITORING AND CONTROLLING PHASE\Testing and Evaluating\Admin PHP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D4DF73-4E9F-4746-AEA0-2AA395CEC2C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,9 +86,6 @@
     <t>Provide valid username/email and password</t>
   </si>
   <si>
-    <t>Trader is redirected to Trader Panel Page</t>
-  </si>
-  <si>
     <t>Invalid Username/Email</t>
   </si>
   <si>
@@ -114,9 +110,6 @@
     <t>Provide empty field in username or password details</t>
   </si>
   <si>
-    <t>Error message is displayed prompting trader to fill out the field</t>
-  </si>
-  <si>
     <t>Forgot Password</t>
   </si>
   <si>
@@ -129,9 +122,6 @@
     <t>Empty Login Fields</t>
   </si>
   <si>
-    <t>An error message is displayed prompting trader to fill out the empty fields</t>
-  </si>
-  <si>
     <t>Admin clicks Sign In button after providing nothing in input fields</t>
   </si>
   <si>
@@ -157,12 +147,21 @@
   </si>
   <si>
     <t>Click on logout button</t>
+  </si>
+  <si>
+    <t>Admin is redirected to Admin Panel Page</t>
+  </si>
+  <si>
+    <t>Error message is displayed prompting Admin to fill out the field</t>
+  </si>
+  <si>
+    <t>An error message is displayed prompting Admin to fill out the empty fields</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -230,9 +229,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -270,9 +269,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -307,7 +306,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -342,7 +341,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -515,11 +514,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -551,13 +550,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -565,13 +564,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
@@ -579,13 +578,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
@@ -593,13 +592,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
         <v>28</v>
       </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
@@ -607,13 +606,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
         <v>31</v>
-      </c>
-      <c r="B7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -621,13 +620,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
@@ -643,10 +642,10 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
         <v>4</v>
@@ -662,7 +661,7 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
@@ -676,7 +675,7 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
@@ -695,7 +694,7 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
         <v>14</v>
@@ -709,10 +708,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
         <v>4</v>
@@ -731,7 +730,7 @@
         <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
         <v>16</v>
@@ -746,7 +745,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -758,7 +757,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Finalized Portfolio and rest
</commit_message>
<xml_diff>
--- a/4.MONITORING AND CONTROLLING PHASE/Testing and Evaluating/Admin PHP/ADMIN PHP TESTING.xlsx
+++ b/4.MONITORING AND CONTROLLING PHASE/Testing and Evaluating/Admin PHP/ADMIN PHP TESTING.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\Portfolio Team Project\Team-Portfolio\4.MONITORING AND CONTROLLING PHASE\Testing and Evaluating\Admin PHP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\Team-Portfolio\4.MONITORING AND CONTROLLING PHASE\Testing and Evaluating\Admin PHP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
   <si>
     <t>TEST CASE</t>
   </si>
@@ -156,6 +156,18 @@
   </si>
   <si>
     <t>An error message is displayed prompting Admin to fill out the empty fields</t>
+  </si>
+  <si>
+    <t>Orders</t>
+  </si>
+  <si>
+    <t>Order History</t>
+  </si>
+  <si>
+    <t>Click on the "Order" Labelled button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin can view all the order history </t>
   </si>
 </sst>
 </file>
@@ -207,10 +219,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -720,27 +733,47 @@
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
     </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>15</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
         <v>41</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C26" t="s">
         <v>16</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D26" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>